<commit_message>
Die Rechnungswerte passen schon!!
</commit_message>
<xml_diff>
--- a/data/Mitgliederliste-Reidlinger.xlsx
+++ b/data/Mitgliederliste-Reidlinger.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21660" windowHeight="3420"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14364" windowHeight="6468"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="48">
   <si>
     <t>Name</t>
   </si>
@@ -257,24 +257,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -313,6 +307,12 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -374,20 +374,20 @@
     <sortCondition ref="A1:A4"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" name="lfd. Nummer" dataDxfId="1"/>
-    <tableColumn id="2" name="Folgezeile" dataDxfId="0"/>
+    <tableColumn id="1" name="lfd. Nummer" dataDxfId="7"/>
+    <tableColumn id="2" name="Folgezeile" dataDxfId="6"/>
     <tableColumn id="14" name="Anrede"/>
     <tableColumn id="3" name="Name"/>
     <tableColumn id="4" name="Vorname"/>
     <tableColumn id="5" name="Adresse"/>
     <tableColumn id="6" name="Stadt"/>
-    <tableColumn id="7" name="Postleitzahl" dataDxfId="7"/>
-    <tableColumn id="8" name="email" dataDxfId="6" dataCellStyle="Link"/>
-    <tableColumn id="9" name="Tel-Nr" dataDxfId="5"/>
+    <tableColumn id="7" name="Postleitzahl" dataDxfId="5"/>
+    <tableColumn id="8" name="email" dataDxfId="4" dataCellStyle="Link"/>
+    <tableColumn id="9" name="Tel-Nr" dataDxfId="3"/>
     <tableColumn id="10" name="Konto"/>
-    <tableColumn id="11" name="Zählpunkt" dataDxfId="4"/>
-    <tableColumn id="12" name="Rabatt" dataDxfId="3"/>
-    <tableColumn id="13" name="Rabatt-Zaehlernummer" dataDxfId="2"/>
+    <tableColumn id="11" name="Zählpunkt" dataDxfId="2"/>
+    <tableColumn id="12" name="Rabatt" dataDxfId="1"/>
+    <tableColumn id="13" name="Rabatt-Zaehlernummer" dataDxfId="0"/>
     <tableColumn id="15" name="Rabatt-Cent"/>
   </tableColumns>
   <tableStyleInfo name="WJ1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -660,8 +660,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -683,14 +683,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -795,7 +795,9 @@
       <c r="A6" s="2">
         <v>1.2</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="C6" s="2"/>
       <c r="H6" s="8"/>
       <c r="I6" s="3"/>
@@ -805,7 +807,7 @@
       <c r="N6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="O6" s="14">
+      <c r="O6" s="12">
         <v>1</v>
       </c>
     </row>
@@ -813,7 +815,9 @@
       <c r="A7" s="2">
         <v>1.3</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="C7" s="2"/>
       <c r="H7" s="8"/>
       <c r="I7" s="3"/>
@@ -823,7 +827,7 @@
       <c r="N7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="O7" s="14">
+      <c r="O7" s="12">
         <v>1</v>
       </c>
     </row>
@@ -831,7 +835,9 @@
       <c r="A8" s="2">
         <v>1.4</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="C8" s="2"/>
       <c r="H8" s="8"/>
       <c r="I8" s="3"/>
@@ -841,7 +847,7 @@
       <c r="N8" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="O8" s="14">
+      <c r="O8" s="12">
         <v>1</v>
       </c>
     </row>
@@ -980,7 +986,7 @@
       <c r="N14" s="5"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="L15" s="13"/>
+      <c r="L15" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>